<commit_message>
fixed a bunch of stuff in heinz
</commit_message>
<xml_diff>
--- a/Projects/HEINZCR/Config/Price Adherence Targets 25Nov2019.xlsx
+++ b/Projects/HEINZCR/Config/Price Adherence Targets 25Nov2019.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="54">
   <si>
     <t xml:space="preserve">EAN CODE</t>
   </si>
@@ -50,9 +50,6 @@
   </si>
   <si>
     <t xml:space="preserve">0735055007042</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0735055007134</t>
   </si>
   <si>
     <t xml:space="preserve">WM</t>
@@ -499,21 +496,21 @@
   <dimension ref="1:116"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I67" activeCellId="0" sqref="I67"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7 A13 A18 A24 A30 A36 A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="29.5612244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="29.1581632653061"/>
     <col collapsed="false" hidden="true" max="6" min="5" style="1" width="0"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="2" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="1020" min="12" style="2" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="1021" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="2" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="1020" min="12" style="2" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1021" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5688,8 +5685,8 @@
       <c r="AMJ6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="s">
-        <v>10</v>
+      <c r="A7" s="7" t="n">
+        <v>735051007134</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>5</v>
@@ -5712,7 +5709,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="8" t="n">
         <v>9</v>
@@ -5732,7 +5729,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="8" t="n">
         <v>9</v>
@@ -5752,7 +5749,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" s="8" t="n">
         <v>9</v>
@@ -5772,7 +5769,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="8" t="n">
         <v>9</v>
@@ -5792,7 +5789,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="8" t="n">
         <v>9</v>
@@ -5808,11 +5805,11 @@
       <c r="K12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="7" t="n">
+        <v>735051007134</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>10</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>11</v>
       </c>
       <c r="C13" s="8" t="n">
         <v>9</v>
@@ -5832,7 +5829,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14" s="8" t="n">
         <v>9</v>
@@ -5852,7 +5849,7 @@
         <v>7</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C15" s="8" t="n">
         <v>9</v>
@@ -5872,7 +5869,7 @@
         <v>8</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C16" s="8" t="n">
         <v>9</v>
@@ -5892,7 +5889,7 @@
         <v>9</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C17" s="8" t="n">
         <v>9</v>
@@ -5908,11 +5905,11 @@
       <c r="K17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7" t="s">
-        <v>10</v>
+      <c r="A18" s="7" t="n">
+        <v>735051007134</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C18" s="8" t="n">
         <v>9</v>
@@ -5932,7 +5929,7 @@
         <v>4</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C19" s="8" t="n">
         <v>9</v>
@@ -5952,7 +5949,7 @@
         <v>6</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C20" s="8" t="n">
         <v>9</v>
@@ -5972,7 +5969,7 @@
         <v>7</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C21" s="8" t="n">
         <v>9</v>
@@ -5992,7 +5989,7 @@
         <v>8</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C22" s="8" t="n">
         <v>9</v>
@@ -6012,7 +6009,7 @@
         <v>9</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C23" s="8" t="n">
         <v>9</v>
@@ -6028,11 +6025,11 @@
       <c r="K23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="7" t="s">
-        <v>10</v>
+      <c r="A24" s="7" t="n">
+        <v>735051007134</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C24" s="8" t="n">
         <v>9</v>
@@ -6052,7 +6049,7 @@
         <v>4</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C25" s="8" t="n">
         <v>9</v>
@@ -6072,7 +6069,7 @@
         <v>6</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C26" s="8" t="n">
         <v>9</v>
@@ -6092,7 +6089,7 @@
         <v>7</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C27" s="8" t="n">
         <v>9</v>
@@ -6112,7 +6109,7 @@
         <v>8</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C28" s="8" t="n">
         <v>9</v>
@@ -6131,7 +6128,7 @@
         <v>9</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C29" s="8" t="n">
         <v>9</v>
@@ -6146,11 +6143,11 @@
       <c r="K29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="7" t="s">
-        <v>10</v>
+      <c r="A30" s="7" t="n">
+        <v>735051007134</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C30" s="8" t="n">
         <v>9</v>
@@ -6169,7 +6166,7 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C31" s="17" t="n">
         <v>9</v>
@@ -6188,7 +6185,7 @@
         <v>6</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C32" s="17" t="n">
         <v>9</v>
@@ -6207,7 +6204,7 @@
         <v>7</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C33" s="17" t="n">
         <v>9</v>
@@ -6226,7 +6223,7 @@
         <v>8</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C34" s="17" t="n">
         <v>9</v>
@@ -6245,7 +6242,7 @@
         <v>9</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C35" s="17" t="n">
         <v>9</v>
@@ -6260,11 +6257,11 @@
       <c r="K35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="16" t="s">
-        <v>10</v>
+      <c r="A36" s="16" t="n">
+        <v>735051007134</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C36" s="17" t="n">
         <v>9</v>
@@ -6283,7 +6280,7 @@
         <v>4</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C37" s="17" t="n">
         <v>9</v>
@@ -6302,7 +6299,7 @@
         <v>6</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C38" s="17" t="n">
         <v>9</v>
@@ -6321,7 +6318,7 @@
         <v>7</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C39" s="17" t="n">
         <v>9</v>
@@ -6340,7 +6337,7 @@
         <v>8</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C40" s="17" t="n">
         <v>9</v>
@@ -6359,7 +6356,7 @@
         <v>9</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C41" s="17" t="n">
         <v>9</v>
@@ -6374,11 +6371,11 @@
       <c r="K41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="16" t="s">
-        <v>10</v>
+      <c r="A42" s="16" t="n">
+        <v>735051007134</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C42" s="17" t="n">
         <v>9</v>
@@ -6394,10 +6391,10 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="C43" s="17" t="n">
         <v>15</v>
@@ -6413,10 +6410,10 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C44" s="17" t="n">
         <v>15</v>
@@ -6432,10 +6429,10 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C45" s="17" t="n">
         <v>15</v>
@@ -6451,10 +6448,10 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C46" s="17" t="n">
         <v>15</v>
@@ -6470,10 +6467,10 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C47" s="17" t="n">
         <v>15</v>
@@ -6489,10 +6486,10 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C48" s="17" t="n">
         <v>15</v>
@@ -6508,10 +6505,10 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C49" s="17" t="n">
         <v>15</v>
@@ -6527,10 +6524,10 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C50" s="17" t="n">
         <v>15</v>
@@ -6546,10 +6543,10 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C51" s="17" t="n">
         <v>15</v>
@@ -6565,10 +6562,10 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="C52" s="17" t="n">
         <v>15</v>
@@ -6584,10 +6581,10 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C53" s="17" t="n">
         <v>15</v>
@@ -6603,10 +6600,10 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C54" s="17" t="n">
         <v>15</v>
@@ -6622,10 +6619,10 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C55" s="17" t="n">
         <v>15</v>
@@ -6641,10 +6638,10 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C56" s="17" t="n">
         <v>15</v>
@@ -6660,10 +6657,10 @@
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C57" s="17" t="n">
         <v>15</v>
@@ -6679,10 +6676,10 @@
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C58" s="17" t="n">
         <v>15</v>
@@ -6698,10 +6695,10 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C59" s="17" t="n">
         <v>15</v>
@@ -6717,10 +6714,10 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C60" s="17" t="n">
         <v>15</v>
@@ -6736,10 +6733,10 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C61" s="17" t="n">
         <v>15</v>
@@ -6755,10 +6752,10 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C62" s="17" t="n">
         <v>15</v>
@@ -6774,10 +6771,10 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C63" s="17" t="n">
         <v>15</v>
@@ -6793,10 +6790,10 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C64" s="17" t="n">
         <v>15</v>
@@ -6812,10 +6809,10 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C65" s="17" t="n">
         <v>15</v>
@@ -6831,10 +6828,10 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C66" s="17" t="n">
         <v>15</v>
@@ -6850,10 +6847,10 @@
     </row>
     <row r="67" customFormat="false" ht="16.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C67" s="17" t="n">
         <v>15</v>
@@ -6869,10 +6866,10 @@
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="C68" s="17" t="n">
         <v>15</v>
@@ -6888,10 +6885,10 @@
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C69" s="17" t="n">
         <v>15</v>
@@ -6907,10 +6904,10 @@
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C70" s="17" t="n">
         <v>15</v>
@@ -6926,10 +6923,10 @@
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C71" s="17" t="n">
         <v>15</v>
@@ -6945,10 +6942,10 @@
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C72" s="17" t="n">
         <v>15</v>
@@ -6964,10 +6961,10 @@
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C73" s="17" t="n">
         <v>15</v>
@@ -6981,10 +6978,10 @@
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C74" s="17" t="n">
         <v>15</v>
@@ -6998,10 +6995,10 @@
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C75" s="17" t="n">
         <v>15</v>
@@ -7015,10 +7012,10 @@
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C76" s="17" t="n">
         <v>15</v>
@@ -7032,10 +7029,10 @@
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="C77" s="17" t="n">
         <v>15</v>
@@ -7049,10 +7046,10 @@
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C78" s="17" t="n">
         <v>15</v>
@@ -7066,10 +7063,10 @@
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C79" s="17" t="n">
         <v>15</v>
@@ -7083,10 +7080,10 @@
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C80" s="17" t="n">
         <v>15</v>
@@ -7100,10 +7097,10 @@
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C81" s="17" t="n">
         <v>15</v>
@@ -7116,10 +7113,10 @@
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C82" s="17" t="n">
         <v>15</v>
@@ -7132,10 +7129,10 @@
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C83" s="17" t="n">
         <v>15</v>
@@ -7148,10 +7145,10 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C84" s="17" t="n">
         <v>15</v>
@@ -7164,10 +7161,10 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C85" s="17" t="n">
         <v>15</v>
@@ -7180,10 +7177,10 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C86" s="17" t="n">
         <v>15</v>
@@ -7196,10 +7193,10 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C87" s="17" t="n">
         <v>15</v>
@@ -7212,10 +7209,10 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C88" s="17" t="n">
         <v>15</v>
@@ -7228,10 +7225,10 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C89" s="17" t="n">
         <v>15</v>
@@ -7244,10 +7241,10 @@
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C90" s="17" t="n">
         <v>15</v>
@@ -7260,10 +7257,10 @@
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C91" s="17" t="n">
         <v>15</v>
@@ -7276,10 +7273,10 @@
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C92" s="17" t="n">
         <v>15</v>
@@ -7295,118 +7292,118 @@
         <v>4</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C93" s="17" t="n">
         <v>10</v>
       </c>
       <c r="D93" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G93" s="0"/>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C94" s="17" t="n">
         <v>10</v>
       </c>
       <c r="D94" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G94" s="0"/>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C95" s="17" t="n">
         <v>10</v>
       </c>
       <c r="D95" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G95" s="0"/>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C96" s="17" t="n">
         <v>10</v>
       </c>
       <c r="D96" s="26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G96" s="0"/>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C97" s="17" t="n">
         <v>10</v>
       </c>
       <c r="D97" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G97" s="0"/>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C98" s="17" t="n">
         <v>10</v>
       </c>
       <c r="D98" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G98" s="0"/>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C99" s="17" t="n">
         <v>10</v>
       </c>
       <c r="D99" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G99" s="0"/>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C100" s="17" t="n">
         <v>10</v>
       </c>
       <c r="D100" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G100" s="0"/>
     </row>
@@ -7415,118 +7412,118 @@
         <v>4</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C101" s="17" t="n">
         <v>10</v>
       </c>
       <c r="D101" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G101" s="0"/>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C102" s="17" t="n">
         <v>10</v>
       </c>
       <c r="D102" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G102" s="0"/>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C103" s="17" t="n">
         <v>10</v>
       </c>
       <c r="D103" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G103" s="0"/>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C104" s="17" t="n">
         <v>10</v>
       </c>
       <c r="D104" s="26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G104" s="0"/>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C105" s="17" t="n">
         <v>10</v>
       </c>
       <c r="D105" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G105" s="0"/>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C106" s="17" t="n">
         <v>10</v>
       </c>
       <c r="D106" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G106" s="0"/>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C107" s="17" t="n">
         <v>10</v>
       </c>
       <c r="D107" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G107" s="0"/>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C108" s="17" t="n">
         <v>10</v>
       </c>
       <c r="D108" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G108" s="0"/>
     </row>
@@ -7535,118 +7532,118 @@
         <v>4</v>
       </c>
       <c r="B109" s="27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C109" s="17" t="n">
         <v>10</v>
       </c>
       <c r="D109" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G109" s="0"/>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B110" s="27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C110" s="17" t="n">
         <v>10</v>
       </c>
       <c r="D110" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G110" s="0"/>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B111" s="27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C111" s="17" t="n">
         <v>10</v>
       </c>
       <c r="D111" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G111" s="0"/>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B112" s="27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C112" s="17" t="n">
         <v>10</v>
       </c>
       <c r="D112" s="26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G112" s="0"/>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B113" s="27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C113" s="17" t="n">
         <v>10</v>
       </c>
       <c r="D113" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G113" s="0"/>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B114" s="27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C114" s="17" t="n">
         <v>10</v>
       </c>
       <c r="D114" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G114" s="0"/>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B115" s="27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C115" s="17" t="n">
         <v>10</v>
       </c>
       <c r="D115" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G115" s="0"/>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B116" s="27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C116" s="17" t="n">
         <v>10</v>
       </c>
       <c r="D116" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G116" s="0"/>
     </row>

</xml_diff>